<commit_message>
Add the product to cart
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/expectedexcelPath.xlsx
+++ b/src/test/resources/excel/expectedexcelPath.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Shopping Portal | Signi-in | Signup</t>
   </si>
@@ -35,6 +34,12 @@
   </si>
   <si>
     <t>Test_Data3</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>Test_Data4</t>
   </si>
 </sst>
 </file>
@@ -380,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -393,7 +398,7 @@
     <col min="4" max="4" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -406,8 +411,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -416,6 +424,9 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>